<commit_message>
UI updates, data fix
</commit_message>
<xml_diff>
--- a/data/total_cholesterol.xlsx
+++ b/data/total_cholesterol.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\DEV\MetaCNMA\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rf174p\Downloads\DEV\MetaCNMA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9ABCAD-463A-4D6D-AF4C-94E7B13BD01F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39AA7858-F369-4EC0-9366-A45583723800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3585" windowWidth="20775" windowHeight="11580" xr2:uid="{0DA68A5C-09B2-4E6E-9DC5-8CB2D8F62A60}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{0DA68A5C-09B2-4E6E-9DC5-8CB2D8F62A60}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -496,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07CA7E63-8C41-4148-951D-1627187840AA}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,7 +670,7 @@
         <v>-0.94</v>
       </c>
       <c r="D10">
-        <v>-0.746</v>
+        <v>0.746</v>
       </c>
       <c r="E10">
         <v>23</v>

</xml_diff>